<commit_message>
Data for Content Modal
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_LIS_Buydown_2022.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_LIS_Buydown_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840D97B5-7B1B-4EA3-9494-1DDBE36B68F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F498A237-6D05-4DC7-A016-AD2511A6F81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="19180" windowHeight="10170" tabRatio="670" activeTab="1" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" firstSheet="4" activeTab="7" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="LIS_Buydown" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="485">
   <si>
     <t>Link Parameters</t>
   </si>
@@ -1516,12 +1516,24 @@
   <si>
     <t>All covered drugs: $0 copay</t>
   </si>
+  <si>
+    <t>During the Coverage Gap Stage, the plan pays all of the cost for your covered drugs.</t>
+  </si>
+  <si>
+    <t>During the Catastrophic Coverage Stage, the plan pays all of the cost for your covered drugs.</t>
+  </si>
+  <si>
+    <t>Initial Coverage Stage Modal</t>
+  </si>
+  <si>
+    <t>During the Initial Coverage Stage, the plan pays all of the cost for your covered drugs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1548,6 +1560,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1569,7 +1588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1582,6 +1601,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6868,15 +6888,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F128AC0-56F7-4ABA-B262-00A33286035D}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="15" max="15" width="55" customWidth="1"/>
+    <col min="16" max="16" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6925,8 +6950,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -6969,14 +6997,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -7019,14 +7050,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -7069,14 +7103,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -7119,14 +7156,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -7169,14 +7209,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -7219,14 +7262,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -7269,14 +7315,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
@@ -7319,14 +7368,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -7369,14 +7421,17 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -7419,14 +7474,17 @@
       <c r="N11" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -7469,14 +7527,17 @@
       <c r="N12" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
@@ -7519,14 +7580,17 @@
       <c r="N13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>98</v>
       </c>
@@ -7569,29 +7633,33 @@
       <c r="N14" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>27</v>
+      <c r="O14" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6DC7FB-338A-43D2-B756-79524782AA33}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7640,8 +7708,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>103</v>
       </c>
@@ -7684,14 +7755,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -7734,14 +7808,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
@@ -7784,14 +7861,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>120</v>
       </c>
@@ -7834,14 +7914,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
@@ -7884,14 +7967,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>127</v>
       </c>
@@ -7934,14 +8020,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -7984,14 +8073,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>135</v>
       </c>
@@ -8034,14 +8126,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
@@ -8084,14 +8179,17 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -8134,14 +8232,17 @@
       <c r="N11" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>159</v>
       </c>
@@ -8184,14 +8285,17 @@
       <c r="N12" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>164</v>
       </c>
@@ -8234,14 +8338,17 @@
       <c r="N13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>171</v>
       </c>
@@ -8284,14 +8391,17 @@
       <c r="N14" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>190</v>
       </c>
@@ -8334,14 +8444,17 @@
       <c r="N15" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>222</v>
       </c>
@@ -8384,14 +8497,17 @@
       <c r="N16" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O16" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>225</v>
       </c>
@@ -8434,11 +8550,14 @@
       <c r="N17" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>27</v>
+      <c r="O17" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -8448,15 +8567,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CBA052-53F9-4CCC-BC00-7A4B98F89442}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="O1" sqref="O1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8505,8 +8624,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>229</v>
       </c>
@@ -8549,14 +8671,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>239</v>
       </c>
@@ -8599,14 +8724,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -8649,14 +8777,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>243</v>
       </c>
@@ -8699,14 +8830,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>245</v>
       </c>
@@ -8749,14 +8883,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>247</v>
       </c>
@@ -8799,14 +8936,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>250</v>
       </c>
@@ -8849,14 +8989,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>256</v>
       </c>
@@ -8899,14 +9042,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>262</v>
       </c>
@@ -8949,14 +9095,17 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>271</v>
       </c>
@@ -8999,14 +9148,17 @@
       <c r="N11" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>275</v>
       </c>
@@ -9049,14 +9201,17 @@
       <c r="N12" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>277</v>
       </c>
@@ -9099,14 +9254,17 @@
       <c r="N13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>283</v>
       </c>
@@ -9149,14 +9307,17 @@
       <c r="N14" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>291</v>
       </c>
@@ -9199,14 +9360,17 @@
       <c r="N15" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>296</v>
       </c>
@@ -9249,11 +9413,14 @@
       <c r="N16" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>27</v>
+      <c r="O16" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -9263,15 +9430,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D489E1FB-3804-4059-9046-85BDC403498E}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9320,8 +9487,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>301</v>
       </c>
@@ -9364,14 +9534,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>304</v>
       </c>
@@ -9414,14 +9587,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>306</v>
       </c>
@@ -9464,14 +9640,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>309</v>
       </c>
@@ -9514,14 +9693,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>311</v>
       </c>
@@ -9564,14 +9746,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>313</v>
       </c>
@@ -9614,14 +9799,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>315</v>
       </c>
@@ -9664,14 +9852,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>318</v>
       </c>
@@ -9714,14 +9905,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>323</v>
       </c>
@@ -9764,14 +9958,17 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>326</v>
       </c>
@@ -9814,14 +10011,17 @@
       <c r="N11" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>329</v>
       </c>
@@ -9864,14 +10064,17 @@
       <c r="N12" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>334</v>
       </c>
@@ -9914,14 +10117,17 @@
       <c r="N13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>337</v>
       </c>
@@ -9964,14 +10170,17 @@
       <c r="N14" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>340</v>
       </c>
@@ -10014,14 +10223,17 @@
       <c r="N15" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>345</v>
       </c>
@@ -10064,11 +10276,14 @@
       <c r="N16" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>27</v>
+      <c r="O16" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -10078,15 +10293,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280623C2-2CB9-46C2-A680-90677F01818E}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="O1" sqref="O1:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10135,8 +10350,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>349</v>
       </c>
@@ -10179,14 +10397,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>355</v>
       </c>
@@ -10229,14 +10450,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>361</v>
       </c>
@@ -10279,14 +10503,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>363</v>
       </c>
@@ -10329,14 +10556,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>367</v>
       </c>
@@ -10379,14 +10609,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>370</v>
       </c>
@@ -10429,14 +10662,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>373</v>
       </c>
@@ -10479,14 +10715,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>379</v>
       </c>
@@ -10529,14 +10768,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>382</v>
       </c>
@@ -10579,14 +10821,17 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>388</v>
       </c>
@@ -10629,14 +10874,17 @@
       <c r="N11" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>390</v>
       </c>
@@ -10679,14 +10927,17 @@
       <c r="N12" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>393</v>
       </c>
@@ -10729,14 +10980,17 @@
       <c r="N13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>396</v>
       </c>
@@ -10779,14 +11033,17 @@
       <c r="N14" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>398</v>
       </c>
@@ -10829,14 +11086,17 @@
       <c r="N15" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>400</v>
       </c>
@@ -10879,11 +11139,14 @@
       <c r="N16" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>27</v>
+      <c r="O16" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -10893,15 +11156,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEB474C-8561-4506-B052-297E8B82B902}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="O1" sqref="O1:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10950,8 +11213,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>402</v>
       </c>
@@ -10994,14 +11260,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>404</v>
       </c>
@@ -11044,14 +11313,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>406</v>
       </c>
@@ -11094,14 +11366,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>411</v>
       </c>
@@ -11144,14 +11419,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>416</v>
       </c>
@@ -11194,14 +11472,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>418</v>
       </c>
@@ -11244,14 +11525,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>421</v>
       </c>
@@ -11294,14 +11578,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>426</v>
       </c>
@@ -11344,14 +11631,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>429</v>
       </c>
@@ -11394,14 +11684,17 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>434</v>
       </c>
@@ -11444,14 +11737,17 @@
       <c r="N11" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>439</v>
       </c>
@@ -11494,14 +11790,17 @@
       <c r="N12" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>442</v>
       </c>
@@ -11544,14 +11843,17 @@
       <c r="N13" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>444</v>
       </c>
@@ -11594,14 +11896,17 @@
       <c r="N14" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>448</v>
       </c>
@@ -11644,14 +11949,17 @@
       <c r="N15" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>450</v>
       </c>
@@ -11694,11 +12002,14 @@
       <c r="N16" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>27</v>
+      <c r="O16" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -11708,15 +12019,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369A45F3-DC0C-4E00-B519-CC5E977ABE10}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11765,8 +12076,11 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>452</v>
       </c>
@@ -11809,14 +12123,17 @@
       <c r="N2" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>454</v>
       </c>
@@ -11859,14 +12176,17 @@
       <c r="N3" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -11909,14 +12229,17 @@
       <c r="N4" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>460</v>
       </c>
@@ -11959,14 +12282,17 @@
       <c r="N5" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>464</v>
       </c>
@@ -12009,14 +12335,17 @@
       <c r="N6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>466</v>
       </c>
@@ -12059,14 +12388,17 @@
       <c r="N7" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>469</v>
       </c>
@@ -12109,14 +12441,17 @@
       <c r="N8" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>472</v>
       </c>
@@ -12159,14 +12494,17 @@
       <c r="N9" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>474</v>
       </c>
@@ -12209,12 +12547,45 @@
       <c r="N10" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="O10" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>